<commit_message>
completed conditional & logical operators in the excel course
</commit_message>
<xml_diff>
--- a/Excel Homework Workbooks/Excel_Homework_Exercises.xlsx
+++ b/Excel Homework Workbooks/Excel_Homework_Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel Homework Workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7545389-70CE-804A-88EB-BD105C5B633E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E0D36-4975-E24E-9C0D-C190C5FC5BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25840" windowHeight="20120" tabRatio="709" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25840" windowHeight="20120" tabRatio="709" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas 101" sheetId="19" r:id="rId1"/>
@@ -5345,7 +5345,7 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -7247,7 +7247,9 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7292,10 +7294,22 @@
       <c r="C2" s="2">
         <v>90</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
+      <c r="D2" s="43" t="str">
+        <f>IF(C2&gt;=60,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E2" s="43" t="str">
+        <f>IF(C2&gt;=90,"A",IF(AND(C2&lt;=89,C2&gt;=80),"B",IF(AND(C2&lt;=79,C2&gt;=70),"C",IF(AND(C2&lt;=69,C2&gt;=60),"D","F"))))</f>
+        <v>A</v>
+      </c>
+      <c r="F2" s="43" t="str">
+        <f>IF(OR(C2&gt;90,C2&lt;60),"OUTLIER","AVG")</f>
+        <v>AVG</v>
+      </c>
+      <c r="G2" s="43" t="str">
+        <f>IF(AND(B2="M",C2&gt;95),"Male Achiever",IF(AND(B2="F",C2&gt;95),"Female Achiever","NONE"))</f>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -7307,10 +7321,22 @@
       <c r="C3" s="2">
         <v>80</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="D3" s="43" t="str">
+        <f t="shared" ref="D3:D16" si="0">IF(C3&gt;=60,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E3" s="43" t="str">
+        <f>IF(C3&gt;=90,"A",IF(AND(C3&lt;=89,C3&gt;=80),"B",IF(AND(C3&lt;=79,C3&gt;=70),"C",IF(AND(C3&lt;=69,C3&gt;=60),"D","F"))))</f>
+        <v>B</v>
+      </c>
+      <c r="F3" s="43" t="str">
+        <f t="shared" ref="F3:F16" si="1">IF(OR(C3&gt;90,C3&lt;60),"OUTLIER","AVG")</f>
+        <v>AVG</v>
+      </c>
+      <c r="G3" s="43" t="str">
+        <f t="shared" ref="G3:G16" si="2">IF(AND(B3="M",C3&gt;95),"Male Achiever",IF(AND(B3="F",C3&gt;95),"Female Achiever","NONE"))</f>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -7322,10 +7348,22 @@
       <c r="C4" s="2">
         <v>96</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="D4" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E4" s="43" t="str">
+        <f>IF(C4&gt;=90,"A",IF(AND(C4&lt;=89,C4&gt;=80),"B",IF(AND(C4&lt;=79,C4&gt;=70),"C",IF(AND(C4&lt;=69,C4&gt;=60),"D","F"))))</f>
+        <v>A</v>
+      </c>
+      <c r="F4" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTLIER</v>
+      </c>
+      <c r="G4" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Female Achiever</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -7337,10 +7375,22 @@
       <c r="C5" s="2">
         <v>72</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
+      <c r="D5" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E5" s="43" t="str">
+        <f>IF(C5&gt;=90,"A",IF(AND(C5&lt;=89,C5&gt;=80),"B",IF(AND(C5&lt;=79,C5&gt;=70),"C",IF(AND(C5&lt;=69,C5&gt;=60),"D","F"))))</f>
+        <v>C</v>
+      </c>
+      <c r="F5" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G5" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -7352,10 +7402,22 @@
       <c r="C6" s="2">
         <v>69</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="D6" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E6" s="43" t="str">
+        <f>IF(C6&gt;=90,"A",IF(AND(C6&lt;=89,C6&gt;=80),"B",IF(AND(C6&lt;=79,C6&gt;=70),"C",IF(AND(C6&lt;=69,C6&gt;=60),"D","F"))))</f>
+        <v>D</v>
+      </c>
+      <c r="F6" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G6" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -7367,10 +7429,22 @@
       <c r="C7" s="2">
         <v>52</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
+      <c r="D7" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="E7" s="43" t="str">
+        <f>IF(C7&gt;=90,"A",IF(AND(C7&lt;=89,C7&gt;=80),"B",IF(AND(C7&lt;=79,C7&gt;=70),"C",IF(AND(C7&lt;=69,C7&gt;=60),"D","F"))))</f>
+        <v>F</v>
+      </c>
+      <c r="F7" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTLIER</v>
+      </c>
+      <c r="G7" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -7382,10 +7456,22 @@
       <c r="C8" s="2">
         <v>99</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="D8" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E8" s="43" t="str">
+        <f t="shared" ref="E8:E16" si="3">IF(C8&gt;=90,"A",IF(AND(C8&lt;=89,C8&gt;=80),"B",IF(AND(C8&lt;=79,C8&gt;=70),"C",IF(AND(C8&lt;=69,C8&gt;=60),"D","F"))))</f>
+        <v>A</v>
+      </c>
+      <c r="F8" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTLIER</v>
+      </c>
+      <c r="G8" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Male Achiever</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -7397,10 +7483,22 @@
       <c r="C9" s="2">
         <v>82</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="D9" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E9" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="F9" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G9" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -7412,10 +7510,22 @@
       <c r="C10" s="2">
         <v>67</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="D10" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E10" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="F10" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G10" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -7427,10 +7537,22 @@
       <c r="C11" s="2">
         <v>90</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="D11" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E11" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+      <c r="F11" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G11" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -7442,10 +7564,22 @@
       <c r="C12" s="2">
         <v>83</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="D12" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E12" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="F12" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G12" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -7457,10 +7591,22 @@
       <c r="C13" s="2">
         <v>89</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="D13" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E13" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="F13" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G13" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -7472,10 +7618,22 @@
       <c r="C14" s="2">
         <v>60</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="D14" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E14" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="F14" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G14" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -7487,10 +7645,22 @@
       <c r="C15" s="2">
         <v>63</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="D15" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E15" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="F15" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>AVG</v>
+      </c>
+      <c r="G15" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -7502,10 +7672,22 @@
       <c r="C16" s="2">
         <v>59</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="D16" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="E16" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="F16" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTLIER</v>
+      </c>
+      <c r="G16" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>NONE</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed statistical functions section and completed the homework assigment for this section
</commit_message>
<xml_diff>
--- a/Excel Homework Workbooks/Excel_Homework_Exercises.xlsx
+++ b/Excel Homework Workbooks/Excel_Homework_Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel Homework Workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E0D36-4975-E24E-9C0D-C190C5FC5BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6266193-F9B5-714D-983B-ECE77EA65524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25840" windowHeight="20120" tabRatio="709" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="20120" tabRatio="709" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas 101" sheetId="19" r:id="rId1"/>
@@ -779,7 +779,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
@@ -787,6 +787,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="m/d;@"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1096,9 +1097,6 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1123,6 +1121,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6111,7 +6112,7 @@
     <col min="3" max="3" width="17.5" style="31" customWidth="1"/>
     <col min="4" max="5" width="14.83203125" style="31" customWidth="1"/>
     <col min="6" max="6" width="24" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="51" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -6133,7 +6134,7 @@
       <c r="F1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="49" t="s">
         <v>131</v>
       </c>
     </row>
@@ -6157,7 +6158,7 @@
       <c r="F2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="52">
+      <c r="G2" s="51">
         <f>E2/B2</f>
         <v>0.41492265696087355</v>
       </c>
@@ -6182,7 +6183,7 @@
       <c r="F3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="52">
         <f t="shared" ref="G3:G25" si="0">E3/B3</f>
         <v>0.17524916943521596</v>
       </c>
@@ -6208,7 +6209,7 @@
       <c r="F4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="52">
         <f t="shared" si="0"/>
         <v>0.50411522633744854</v>
       </c>
@@ -6234,7 +6235,7 @@
       <c r="F5" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="52">
         <f t="shared" si="0"/>
         <v>0.52380952380952384</v>
       </c>
@@ -6260,7 +6261,7 @@
       <c r="F6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="52">
         <f t="shared" si="0"/>
         <v>0.43443132380360472</v>
       </c>
@@ -6286,7 +6287,7 @@
       <c r="F7" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="52">
         <f t="shared" si="0"/>
         <v>0.39156626506024095</v>
       </c>
@@ -6312,7 +6313,7 @@
       <c r="F8" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G8" s="53">
+      <c r="G8" s="52">
         <f t="shared" si="0"/>
         <v>0.57631444614599281</v>
       </c>
@@ -6338,7 +6339,7 @@
       <c r="F9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="52">
         <f t="shared" si="0"/>
         <v>0.51498929336188437</v>
       </c>
@@ -6364,7 +6365,7 @@
       <c r="F10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="52">
         <f t="shared" si="0"/>
         <v>0.47848537005163511</v>
       </c>
@@ -6390,7 +6391,7 @@
       <c r="F11" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="52">
         <f t="shared" si="0"/>
         <v>0.3377808988764045</v>
       </c>
@@ -6416,7 +6417,7 @@
       <c r="F12" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="52">
         <f t="shared" si="0"/>
         <v>0.34983766233766234</v>
       </c>
@@ -6442,7 +6443,7 @@
       <c r="F13" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="52">
         <f t="shared" si="0"/>
         <v>0.54775604142692746</v>
       </c>
@@ -6468,7 +6469,7 @@
       <c r="F14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="52">
         <f t="shared" si="0"/>
         <v>0.5993031358885017</v>
       </c>
@@ -6494,7 +6495,7 @@
       <c r="F15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="52">
         <f t="shared" si="0"/>
         <v>0.59571045576407511</v>
       </c>
@@ -6520,7 +6521,7 @@
       <c r="F16" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="53">
+      <c r="G16" s="52">
         <f t="shared" si="0"/>
         <v>0.51458670988654787</v>
       </c>
@@ -6546,7 +6547,7 @@
       <c r="F17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="53">
+      <c r="G17" s="52">
         <f t="shared" si="0"/>
         <v>0.40393151553582751</v>
       </c>
@@ -6572,7 +6573,7 @@
       <c r="F18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="52">
         <f t="shared" si="0"/>
         <v>0.51891074130105896</v>
       </c>
@@ -6598,7 +6599,7 @@
       <c r="F19" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="52">
         <f t="shared" si="0"/>
         <v>0.57448377581120946</v>
       </c>
@@ -6623,7 +6624,7 @@
       <c r="F20" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="52">
         <f t="shared" si="0"/>
         <v>0.47118463180362863</v>
       </c>
@@ -6649,7 +6650,7 @@
       <c r="F21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="52">
         <f t="shared" si="0"/>
         <v>0.60243407707910746</v>
       </c>
@@ -6674,7 +6675,7 @@
       <c r="F22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G22" s="53">
+      <c r="G22" s="52">
         <f t="shared" si="0"/>
         <v>0.36644364384971695</v>
       </c>
@@ -6700,7 +6701,7 @@
       <c r="F23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G23" s="53">
+      <c r="G23" s="52">
         <f t="shared" si="0"/>
         <v>0.54501385041551242</v>
       </c>
@@ -6726,7 +6727,7 @@
       <c r="F24" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G24" s="53">
+      <c r="G24" s="52">
         <f t="shared" si="0"/>
         <v>0.4105827193569993</v>
       </c>
@@ -6752,7 +6753,7 @@
       <c r="F25" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G25" s="53">
+      <c r="G25" s="52">
         <f t="shared" si="0"/>
         <v>0.66628308400460301</v>
       </c>
@@ -6807,19 +6808,19 @@
       <c r="E1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="53" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6892,10 +6893,10 @@
       <c r="I4" s="2"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="M4" s="54" t="s">
+      <c r="M4" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="N4" s="54" t="s">
+      <c r="N4" s="53" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6939,7 +6940,7 @@
       <c r="E6" s="8">
         <v>10283</v>
       </c>
-      <c r="G6" s="55"/>
+      <c r="G6" s="54"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="8"/>
@@ -6963,7 +6964,7 @@
       <c r="E7" s="8">
         <v>15332</v>
       </c>
-      <c r="G7" s="55"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
@@ -6993,7 +6994,7 @@
       <c r="M8" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="N8" s="56" t="s">
+      <c r="N8" s="55" t="s">
         <v>212</v>
       </c>
     </row>
@@ -7040,19 +7041,19 @@
       <c r="I10" s="2"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="M10" s="54" t="s">
+      <c r="M10" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="N10" s="54" t="s">
+      <c r="N10" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="O10" s="54" t="s">
+      <c r="O10" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="P10" s="54" t="s">
+      <c r="P10" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="Q10" s="54" t="s">
+      <c r="Q10" s="53" t="s">
         <v>210</v>
       </c>
     </row>
@@ -7209,10 +7210,10 @@
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M17" s="54" t="s">
+      <c r="M17" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="N17" s="54" t="s">
+      <c r="N17" s="53" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7247,7 +7248,7 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -7299,7 +7300,7 @@
         <v>PASS</v>
       </c>
       <c r="E2" s="43" t="str">
-        <f>IF(C2&gt;=90,"A",IF(AND(C2&lt;=89,C2&gt;=80),"B",IF(AND(C2&lt;=79,C2&gt;=70),"C",IF(AND(C2&lt;=69,C2&gt;=60),"D","F"))))</f>
+        <f t="shared" ref="E2:E7" si="0">IF(C2&gt;=90,"A",IF(AND(C2&lt;=89,C2&gt;=80),"B",IF(AND(C2&lt;=79,C2&gt;=70),"C",IF(AND(C2&lt;=69,C2&gt;=60),"D","F"))))</f>
         <v>A</v>
       </c>
       <c r="F2" s="43" t="str">
@@ -7322,19 +7323,19 @@
         <v>80</v>
       </c>
       <c r="D3" s="43" t="str">
-        <f t="shared" ref="D3:D16" si="0">IF(C3&gt;=60,"PASS","FAIL")</f>
+        <f t="shared" ref="D3:D16" si="1">IF(C3&gt;=60,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="E3" s="43" t="str">
-        <f>IF(C3&gt;=90,"A",IF(AND(C3&lt;=89,C3&gt;=80),"B",IF(AND(C3&lt;=79,C3&gt;=70),"C",IF(AND(C3&lt;=69,C3&gt;=60),"D","F"))))</f>
+        <f t="shared" si="0"/>
         <v>B</v>
       </c>
       <c r="F3" s="43" t="str">
-        <f t="shared" ref="F3:F16" si="1">IF(OR(C3&gt;90,C3&lt;60),"OUTLIER","AVG")</f>
+        <f t="shared" ref="F3:F16" si="2">IF(OR(C3&gt;90,C3&lt;60),"OUTLIER","AVG")</f>
         <v>AVG</v>
       </c>
       <c r="G3" s="43" t="str">
-        <f t="shared" ref="G3:G16" si="2">IF(AND(B3="M",C3&gt;95),"Male Achiever",IF(AND(B3="F",C3&gt;95),"Female Achiever","NONE"))</f>
+        <f t="shared" ref="G3:G16" si="3">IF(AND(B3="M",C3&gt;95),"Male Achiever",IF(AND(B3="F",C3&gt;95),"Female Achiever","NONE"))</f>
         <v>NONE</v>
       </c>
     </row>
@@ -7349,19 +7350,19 @@
         <v>96</v>
       </c>
       <c r="D4" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E4" s="43" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E4" s="43" t="str">
-        <f>IF(C4&gt;=90,"A",IF(AND(C4&lt;=89,C4&gt;=80),"B",IF(AND(C4&lt;=79,C4&gt;=70),"C",IF(AND(C4&lt;=69,C4&gt;=60),"D","F"))))</f>
         <v>A</v>
       </c>
       <c r="F4" s="43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>OUTLIER</v>
       </c>
       <c r="G4" s="43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Female Achiever</v>
       </c>
     </row>
@@ -7376,19 +7377,19 @@
         <v>72</v>
       </c>
       <c r="D5" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E5" s="43" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E5" s="43" t="str">
-        <f>IF(C5&gt;=90,"A",IF(AND(C5&lt;=89,C5&gt;=80),"B",IF(AND(C5&lt;=79,C5&gt;=70),"C",IF(AND(C5&lt;=69,C5&gt;=60),"D","F"))))</f>
         <v>C</v>
       </c>
       <c r="F5" s="43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>AVG</v>
       </c>
       <c r="G5" s="43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7403,19 +7404,19 @@
         <v>69</v>
       </c>
       <c r="D6" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E6" s="43" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E6" s="43" t="str">
-        <f>IF(C6&gt;=90,"A",IF(AND(C6&lt;=89,C6&gt;=80),"B",IF(AND(C6&lt;=79,C6&gt;=70),"C",IF(AND(C6&lt;=69,C6&gt;=60),"D","F"))))</f>
         <v>D</v>
       </c>
       <c r="F6" s="43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>AVG</v>
       </c>
       <c r="G6" s="43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7430,19 +7431,19 @@
         <v>52</v>
       </c>
       <c r="D7" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+      <c r="E7" s="43" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
-      </c>
-      <c r="E7" s="43" t="str">
-        <f>IF(C7&gt;=90,"A",IF(AND(C7&lt;=89,C7&gt;=80),"B",IF(AND(C7&lt;=79,C7&gt;=70),"C",IF(AND(C7&lt;=69,C7&gt;=60),"D","F"))))</f>
         <v>F</v>
       </c>
       <c r="F7" s="43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>OUTLIER</v>
       </c>
       <c r="G7" s="43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7457,19 +7458,19 @@
         <v>99</v>
       </c>
       <c r="D8" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E8" s="43" t="str">
-        <f t="shared" ref="E8:E16" si="3">IF(C8&gt;=90,"A",IF(AND(C8&lt;=89,C8&gt;=80),"B",IF(AND(C8&lt;=79,C8&gt;=70),"C",IF(AND(C8&lt;=69,C8&gt;=60),"D","F"))))</f>
+        <f t="shared" ref="E8:E16" si="4">IF(C8&gt;=90,"A",IF(AND(C8&lt;=89,C8&gt;=80),"B",IF(AND(C8&lt;=79,C8&gt;=70),"C",IF(AND(C8&lt;=69,C8&gt;=60),"D","F"))))</f>
         <v>A</v>
       </c>
       <c r="F8" s="43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>OUTLIER</v>
       </c>
       <c r="G8" s="43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Male Achiever</v>
       </c>
     </row>
@@ -7484,19 +7485,19 @@
         <v>82</v>
       </c>
       <c r="D9" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E9" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="F9" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>AVG</v>
+      </c>
+      <c r="G9" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>B</v>
-      </c>
-      <c r="F9" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>AVG</v>
-      </c>
-      <c r="G9" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7511,19 +7512,19 @@
         <v>67</v>
       </c>
       <c r="D10" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E10" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+      <c r="F10" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>AVG</v>
+      </c>
+      <c r="G10" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>D</v>
-      </c>
-      <c r="F10" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>AVG</v>
-      </c>
-      <c r="G10" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7538,19 +7539,19 @@
         <v>90</v>
       </c>
       <c r="D11" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E11" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>A</v>
+      </c>
+      <c r="F11" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>AVG</v>
+      </c>
+      <c r="G11" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>A</v>
-      </c>
-      <c r="F11" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>AVG</v>
-      </c>
-      <c r="G11" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7565,19 +7566,19 @@
         <v>83</v>
       </c>
       <c r="D12" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E12" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="F12" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>AVG</v>
+      </c>
+      <c r="G12" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>B</v>
-      </c>
-      <c r="F12" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>AVG</v>
-      </c>
-      <c r="G12" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7592,19 +7593,19 @@
         <v>89</v>
       </c>
       <c r="D13" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E13" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="F13" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>AVG</v>
+      </c>
+      <c r="G13" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>B</v>
-      </c>
-      <c r="F13" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>AVG</v>
-      </c>
-      <c r="G13" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7619,19 +7620,19 @@
         <v>60</v>
       </c>
       <c r="D14" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E14" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+      <c r="F14" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>AVG</v>
+      </c>
+      <c r="G14" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>D</v>
-      </c>
-      <c r="F14" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>AVG</v>
-      </c>
-      <c r="G14" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7646,19 +7647,19 @@
         <v>63</v>
       </c>
       <c r="D15" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PASS</v>
       </c>
       <c r="E15" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+      <c r="F15" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>AVG</v>
+      </c>
+      <c r="G15" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>D</v>
-      </c>
-      <c r="F15" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>AVG</v>
-      </c>
-      <c r="G15" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7673,19 +7674,19 @@
         <v>59</v>
       </c>
       <c r="D16" s="43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>FAIL</v>
       </c>
       <c r="E16" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+      <c r="F16" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>OUTLIER</v>
+      </c>
+      <c r="G16" s="43" t="str">
         <f t="shared" si="3"/>
-        <v>F</v>
-      </c>
-      <c r="F16" s="43" t="str">
-        <f t="shared" si="1"/>
-        <v>OUTLIER</v>
-      </c>
-      <c r="G16" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NONE</v>
       </c>
     </row>
@@ -7702,7 +7703,9 @@
   </sheetPr>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7760,7 +7763,7 @@
         <v>117</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>118</v>
@@ -7827,7 +7830,10 @@
       <c r="E5" s="8">
         <v>3072</v>
       </c>
-      <c r="H5" s="36"/>
+      <c r="H5" s="36">
+        <f>SUMIF(A:A,$H$2,D:D)</f>
+        <v>3325</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -7891,9 +7897,18 @@
       <c r="G8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="36"/>
+      <c r="H8" s="36">
+        <f>SUMIFS($D:$D,$C:$C,$G8,$A:$A,$H$2)</f>
+        <v>1080</v>
+      </c>
+      <c r="I8" s="56">
+        <f>SUMIFS($E:$E,$C:$C,G8,A:A,$H$2)</f>
+        <v>96137</v>
+      </c>
+      <c r="J8" s="36">
+        <f>COUNTIFS(C:C,G8,A:A,$H$2)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -7914,9 +7929,18 @@
       <c r="G9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="36"/>
+      <c r="H9" s="36">
+        <f t="shared" ref="H9:H10" si="0">SUMIFS($D:$D,$C:$C,G9,A:A,$H$2)</f>
+        <v>1568</v>
+      </c>
+      <c r="I9" s="56">
+        <f t="shared" ref="I9:I10" si="1">SUMIFS($E:$E,$C:$C,G9,A:A,$H$2)</f>
+        <v>97796</v>
+      </c>
+      <c r="J9" s="36">
+        <f t="shared" ref="J9:J10" si="2">COUNTIFS(C:C,G9,A:A,$H$2)</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -7937,9 +7961,18 @@
       <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="36"/>
+      <c r="H10" s="36">
+        <f t="shared" si="0"/>
+        <v>677</v>
+      </c>
+      <c r="I10" s="56">
+        <f t="shared" si="1"/>
+        <v>41514</v>
+      </c>
+      <c r="J10" s="36">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -14858,7 +14891,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.83203125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="48" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
@@ -14868,7 +14901,7 @@
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>204</v>
       </c>
       <c r="C1" s="19" t="s">
@@ -14944,7 +14977,7 @@
       <c r="F5" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">

</xml_diff>

<commit_message>
completed section 9 dynamic array formulas
</commit_message>
<xml_diff>
--- a/Excel Homework Workbooks/Excel_Homework_Exercises.xlsx
+++ b/Excel Homework Workbooks/Excel_Homework_Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel Homework Workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9931C058-FA33-124E-B8E9-66A8C83C4D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40B5F41-B606-3045-B297-97754303EA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27600" windowHeight="20120" tabRatio="709" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28320" windowHeight="20120" tabRatio="709" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas 101" sheetId="19" r:id="rId1"/>
@@ -48,6 +48,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="234">
   <si>
@@ -789,8 +811,8 @@
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="m/d;@"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="dddd"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="dddd"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1115,19 +1137,19 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1144,7 +1166,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1162,224 +1184,6 @@
         <u val="none"/>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u val="none"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6226,7 +6030,7 @@
       </c>
       <c r="C3" s="37">
         <f ca="1">TODAY()</f>
-        <v>44955</v>
+        <v>44957</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6235,7 +6039,7 @@
       </c>
       <c r="C4" s="38">
         <f ca="1">NOW()</f>
-        <v>44955.879836921296</v>
+        <v>44957.610915046294</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6269,19 +6073,19 @@
       </c>
       <c r="D7" s="39">
         <f ca="1">DAY($C$4)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E7" s="39">
         <f ca="1">HOUR($C$4)</f>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F7" s="39">
         <f ca="1">MINUTE($C$4)</f>
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G7" s="39">
         <f ca="1">SECOND($C$4)</f>
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6299,7 +6103,7 @@
       </c>
       <c r="C9" s="52">
         <f ca="1">WEEKDAY(C3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6312,7 +6116,7 @@
       </c>
       <c r="C11" s="37">
         <f ca="1">WORKDAY(C3,50)</f>
-        <v>45023</v>
+        <v>45027</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6321,7 +6125,7 @@
       </c>
       <c r="C12" s="40">
         <f ca="1">NETWORKDAYS(C2,C3)</f>
-        <v>2107</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -6402,7 +6206,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -6472,7 +6276,7 @@
         <v>1204</v>
       </c>
       <c r="C3" s="54">
-        <f>B3-B2</f>
+        <f t="shared" ref="C3:C25" si="0">B3-B2</f>
         <v>105</v>
       </c>
       <c r="D3" s="54">
@@ -6485,7 +6289,7 @@
         <v>133</v>
       </c>
       <c r="G3" s="58">
-        <f t="shared" ref="G3:G25" si="0">E3/B3</f>
+        <f t="shared" ref="G3:G25" si="1">E3/B3</f>
         <v>0.17524916943521596</v>
       </c>
     </row>
@@ -6497,21 +6301,21 @@
         <v>1944</v>
       </c>
       <c r="C4" s="54">
-        <f>B4-B3</f>
+        <f t="shared" si="0"/>
         <v>740</v>
       </c>
       <c r="D4" s="54">
         <v>964</v>
       </c>
       <c r="E4" s="54">
-        <f t="shared" ref="E4:E25" si="1">B4-D4</f>
+        <f t="shared" ref="E4:E25" si="2">B4-D4</f>
         <v>980</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G4" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.50411522633744854</v>
       </c>
     </row>
@@ -6523,21 +6327,21 @@
         <v>1743</v>
       </c>
       <c r="C5" s="54">
-        <f>B5-B4</f>
+        <f t="shared" si="0"/>
         <v>-201</v>
       </c>
       <c r="D5" s="54">
         <v>830</v>
       </c>
       <c r="E5" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>913</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G5" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.52380952380952384</v>
       </c>
     </row>
@@ -6549,21 +6353,21 @@
         <v>1609</v>
       </c>
       <c r="C6" s="54">
-        <f>B6-B5</f>
+        <f t="shared" si="0"/>
         <v>-134</v>
       </c>
       <c r="D6" s="54">
         <v>910</v>
       </c>
       <c r="E6" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>699</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G6" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.43443132380360472</v>
       </c>
     </row>
@@ -6575,21 +6379,21 @@
         <v>1494</v>
       </c>
       <c r="C7" s="54">
-        <f>B7-B6</f>
+        <f t="shared" si="0"/>
         <v>-115</v>
       </c>
       <c r="D7" s="54">
         <v>909</v>
       </c>
       <c r="E7" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>585</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G7" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.39156626506024095</v>
       </c>
     </row>
@@ -6601,21 +6405,21 @@
         <v>1959</v>
       </c>
       <c r="C8" s="54">
-        <f>B8-B7</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
       <c r="D8" s="54">
         <v>830</v>
       </c>
       <c r="E8" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1129</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G8" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.57631444614599281</v>
       </c>
     </row>
@@ -6627,21 +6431,21 @@
         <v>1868</v>
       </c>
       <c r="C9" s="54">
-        <f>B9-B8</f>
+        <f t="shared" si="0"/>
         <v>-91</v>
       </c>
       <c r="D9" s="54">
         <v>906</v>
       </c>
       <c r="E9" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>962</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G9" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.51498929336188437</v>
       </c>
     </row>
@@ -6653,21 +6457,21 @@
         <v>1162</v>
       </c>
       <c r="C10" s="54">
-        <f>B10-B9</f>
+        <f t="shared" si="0"/>
         <v>-706</v>
       </c>
       <c r="D10" s="54">
         <v>606</v>
       </c>
       <c r="E10" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>556</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G10" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.47848537005163511</v>
       </c>
     </row>
@@ -6679,21 +6483,21 @@
         <v>1424</v>
       </c>
       <c r="C11" s="54">
-        <f>B11-B10</f>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="D11" s="54">
         <v>943</v>
       </c>
       <c r="E11" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>481</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G11" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3377808988764045</v>
       </c>
     </row>
@@ -6705,21 +6509,21 @@
         <v>1232</v>
       </c>
       <c r="C12" s="54">
-        <f>B12-B11</f>
+        <f t="shared" si="0"/>
         <v>-192</v>
       </c>
       <c r="D12" s="54">
         <v>801</v>
       </c>
       <c r="E12" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>431</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G12" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34983766233766234</v>
       </c>
     </row>
@@ -6731,21 +6535,21 @@
         <v>1738</v>
       </c>
       <c r="C13" s="54">
-        <f>B13-B12</f>
+        <f t="shared" si="0"/>
         <v>506</v>
       </c>
       <c r="D13" s="54">
         <v>786</v>
       </c>
       <c r="E13" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>952</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G13" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.54775604142692746</v>
       </c>
     </row>
@@ -6757,21 +6561,21 @@
         <v>1435</v>
       </c>
       <c r="C14" s="54">
-        <f>B14-B13</f>
+        <f t="shared" si="0"/>
         <v>-303</v>
       </c>
       <c r="D14" s="54">
         <v>575</v>
       </c>
       <c r="E14" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>860</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G14" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5993031358885017</v>
       </c>
     </row>
@@ -6783,21 +6587,21 @@
         <v>1865</v>
       </c>
       <c r="C15" s="54">
-        <f>B15-B14</f>
+        <f t="shared" si="0"/>
         <v>430</v>
       </c>
       <c r="D15" s="54">
         <v>754</v>
       </c>
       <c r="E15" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1111</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G15" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59571045576407511</v>
       </c>
     </row>
@@ -6809,21 +6613,21 @@
         <v>1234</v>
       </c>
       <c r="C16" s="54">
-        <f>B16-B15</f>
+        <f t="shared" si="0"/>
         <v>-631</v>
       </c>
       <c r="D16" s="54">
         <v>599</v>
       </c>
       <c r="E16" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>635</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G16" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.51458670988654787</v>
       </c>
     </row>
@@ -6835,21 +6639,21 @@
         <v>1577</v>
       </c>
       <c r="C17" s="54">
-        <f>B17-B16</f>
+        <f t="shared" si="0"/>
         <v>343</v>
       </c>
       <c r="D17" s="54">
         <v>940</v>
       </c>
       <c r="E17" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>637</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G17" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40393151553582751</v>
       </c>
     </row>
@@ -6861,21 +6665,21 @@
         <v>1983</v>
       </c>
       <c r="C18" s="54">
-        <f>B18-B17</f>
+        <f t="shared" si="0"/>
         <v>406</v>
       </c>
       <c r="D18" s="54">
         <v>954</v>
       </c>
       <c r="E18" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1029</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G18" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.51891074130105896</v>
       </c>
     </row>
@@ -6887,21 +6691,21 @@
         <v>1356</v>
       </c>
       <c r="C19" s="54">
-        <f>B19-B18</f>
+        <f t="shared" si="0"/>
         <v>-627</v>
       </c>
       <c r="D19" s="54">
         <v>577</v>
       </c>
       <c r="E19" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>779</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G19" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.57448377581120946</v>
       </c>
     </row>
@@ -6913,7 +6717,7 @@
         <v>1874</v>
       </c>
       <c r="C20" s="54">
-        <f>B20-B19</f>
+        <f t="shared" si="0"/>
         <v>518</v>
       </c>
       <c r="D20" s="54">
@@ -6926,7 +6730,7 @@
         <v>133</v>
       </c>
       <c r="G20" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.47118463180362863</v>
       </c>
     </row>
@@ -6938,21 +6742,21 @@
         <v>1479</v>
       </c>
       <c r="C21" s="54">
-        <f>B21-B20</f>
+        <f t="shared" si="0"/>
         <v>-395</v>
       </c>
       <c r="D21" s="54">
         <v>588</v>
       </c>
       <c r="E21" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>891</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G21" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.60243407707910746</v>
       </c>
     </row>
@@ -6964,7 +6768,7 @@
         <v>1943</v>
       </c>
       <c r="C22" s="54">
-        <f>B22-B21</f>
+        <f t="shared" si="0"/>
         <v>464</v>
       </c>
       <c r="D22" s="54">
@@ -6977,7 +6781,7 @@
         <v>133</v>
       </c>
       <c r="G22" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.36644364384971695</v>
       </c>
     </row>
@@ -6989,21 +6793,21 @@
         <v>1444</v>
       </c>
       <c r="C23" s="54">
-        <f>B23-B22</f>
+        <f t="shared" si="0"/>
         <v>-499</v>
       </c>
       <c r="D23" s="54">
         <v>657</v>
       </c>
       <c r="E23" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>787</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G23" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.54501385041551242</v>
       </c>
     </row>
@@ -7015,21 +6819,21 @@
         <v>1493</v>
       </c>
       <c r="C24" s="54">
-        <f>B24-B23</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="D24" s="54">
         <v>880</v>
       </c>
       <c r="E24" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>613</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G24" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4105827193569993</v>
       </c>
     </row>
@@ -7041,21 +6845,21 @@
         <v>1738</v>
       </c>
       <c r="C25" s="54">
-        <f>B25-B24</f>
+        <f t="shared" si="0"/>
         <v>245</v>
       </c>
       <c r="D25" s="54">
         <v>580</v>
       </c>
       <c r="E25" s="54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1158</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G25" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.66628308400460301</v>
       </c>
     </row>
@@ -7073,12 +6877,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A25">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>G2&lt;0.4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F25">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$F2="Kids"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7119,8 +6923,8 @@
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7188,15 +6992,29 @@
       <c r="E2" s="8">
         <v>22873</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="G2" s="42" t="str" cm="1">
+        <f t="array" ref="G2:K16">_xlfn._xlws.SORT(A2:E16,{2,5},{1,-1})</f>
+        <v>Kathy</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <v>BOS</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J2" s="8">
+        <v>18270</v>
+      </c>
+      <c r="K2" s="8">
+        <v>22873</v>
+      </c>
       <c r="M2" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="N2" s="39"/>
+      <c r="N2" s="39" t="str" cm="1">
+        <f t="array" ref="N2">_xlfn._xlws.FILTER(A2:A16,E2:E16=MAX(E2:E16))</f>
+        <v>Sam</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -7214,11 +7032,21 @@
       <c r="E3" s="8">
         <v>21279</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="G3" s="2" t="str">
+        <v>John</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <v>BOS</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J3" s="8">
+        <v>20510</v>
+      </c>
+      <c r="K3" s="8">
+        <v>21279</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -7236,11 +7064,21 @@
       <c r="E4" s="8">
         <v>13096</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="G4" s="2" t="str">
+        <v>Mindy</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <v>BOS</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="J4" s="8">
+        <v>15972</v>
+      </c>
+      <c r="K4" s="8">
+        <v>13096</v>
+      </c>
       <c r="M4" s="48" t="s">
         <v>208</v>
       </c>
@@ -7264,13 +7102,29 @@
       <c r="E5" s="8">
         <v>10990</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="41"/>
+      <c r="G5" s="2" t="str">
+        <v>Aaron</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <v>BOS</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="J5" s="8">
+        <v>17347</v>
+      </c>
+      <c r="K5" s="8">
+        <v>10990</v>
+      </c>
+      <c r="M5" s="42" t="str" cm="1">
+        <f t="array" ref="M5:M6">_xlfn._xlws.SORT(_xlfn.UNIQUE(C2:C16))</f>
+        <v>Apparel</v>
+      </c>
+      <c r="N5" s="41" cm="1">
+        <f t="array" ref="N5:N6">SUMIFS(E2:E16,C2:C16,_xlfn.ANCHORARRAY(M5))</f>
+        <v>136990</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -7288,13 +7142,27 @@
       <c r="E6" s="8">
         <v>10283</v>
       </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="8"/>
+      <c r="G6" s="49" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <v>CHI</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="J6" s="8">
+        <v>26508</v>
+      </c>
+      <c r="K6" s="8">
+        <v>28682</v>
+      </c>
+      <c r="M6" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="N6" s="8">
+        <v>162245</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -7312,11 +7180,21 @@
       <c r="E7" s="8">
         <v>15332</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="G7" s="49" t="str">
+        <v>Jean</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <v>CHI</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J7" s="8">
+        <v>23810</v>
+      </c>
+      <c r="K7" s="8">
+        <v>28543</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -7334,16 +7212,26 @@
       <c r="E8" s="8">
         <v>15414</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="G8" s="2" t="str">
+        <v>Tina</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <v>CHI</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J8" s="8">
+        <v>19325</v>
+      </c>
+      <c r="K8" s="8">
+        <v>26697</v>
+      </c>
       <c r="M8" s="9" t="s">
         <v>231</v>
       </c>
       <c r="N8" s="50" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -7362,11 +7250,21 @@
       <c r="E9" s="8">
         <v>21973</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="G9" s="2" t="str">
+        <v>Kim</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <v>CHI</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J9" s="8">
+        <v>29120</v>
+      </c>
+      <c r="K9" s="8">
+        <v>21824</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -7384,11 +7282,21 @@
       <c r="E10" s="8">
         <v>18721</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="G10" s="2" t="str">
+        <v>Ashley</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <v>CHI</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="J10" s="8">
+        <v>17872</v>
+      </c>
+      <c r="K10" s="8">
+        <v>17631</v>
+      </c>
       <c r="M10" s="48" t="s">
         <v>206</v>
       </c>
@@ -7421,16 +7329,37 @@
       <c r="E11" s="8">
         <v>25897</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="G11" s="2" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="H11" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="J11" s="8">
+        <v>25347</v>
+      </c>
+      <c r="K11" s="8">
+        <v>25897</v>
+      </c>
+      <c r="M11" s="42" t="str" cm="1">
+        <f t="array" ref="M11:Q14">_xlfn._xlws.FILTER(A2:E16,(B2:B16=N8)*(D2:D16&lt;E2:E16))</f>
+        <v>Tom</v>
+      </c>
+      <c r="N11" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="P11" s="8">
+        <v>13190</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>15332</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -7448,16 +7377,36 @@
       <c r="E12" s="8">
         <v>21824</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="G12" s="2" t="str">
+        <v>Lauren</v>
+      </c>
+      <c r="H12" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="J12" s="8">
+        <v>19588</v>
+      </c>
+      <c r="K12" s="8">
+        <v>21973</v>
+      </c>
+      <c r="M12" s="2" t="str">
+        <v>Lauren</v>
+      </c>
+      <c r="N12" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="P12" s="8">
+        <v>19588</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>21973</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -7475,16 +7424,36 @@
       <c r="E13" s="8">
         <v>26697</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
+      <c r="G13" s="2" t="str">
+        <v>Jason</v>
+      </c>
+      <c r="H13" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="J13" s="8">
+        <v>15769</v>
+      </c>
+      <c r="K13" s="8">
+        <v>18721</v>
+      </c>
+      <c r="M13" s="2" t="str">
+        <v>Jason</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="P13" s="8">
+        <v>15769</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>18721</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -7502,16 +7471,36 @@
       <c r="E14" s="8">
         <v>28543</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
+      <c r="G14" s="2" t="str">
+        <v>Bill</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J14" s="8">
+        <v>17585</v>
+      </c>
+      <c r="K14" s="8">
+        <v>15414</v>
+      </c>
+      <c r="M14" s="2" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="O14" s="2" t="str">
+        <v>Apparel</v>
+      </c>
+      <c r="P14" s="8">
+        <v>25347</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>25897</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -7529,11 +7518,21 @@
       <c r="E15" s="8">
         <v>28682</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="G15" s="2" t="str">
+        <v>Tom</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J15" s="8">
+        <v>13190</v>
+      </c>
+      <c r="K15" s="8">
+        <v>15332</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -7551,11 +7550,21 @@
       <c r="E16" s="8">
         <v>17631</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="G16" s="2" t="str">
+        <v>Phil</v>
+      </c>
+      <c r="H16" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="J16" s="8">
+        <v>19635</v>
+      </c>
+      <c r="K16" s="8">
+        <v>10283</v>
+      </c>
     </row>
     <row r="17" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M17" s="48" t="s">
@@ -7566,16 +7575,34 @@
       </c>
     </row>
     <row r="18" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M18" s="42"/>
-      <c r="N18" s="30"/>
+      <c r="M18" s="42" t="str" cm="1">
+        <f t="array" ref="M18:N20">_xlfn.LET(_xlpm.office,_xlfn.UNIQUE(B2:B16),
+_xlpm.sales2015,SUMIFS(D2:D16,B2:B16,_xlpm.office),
+_xlpm.sales2016,SUMIFS(E2:E16,B2:B16,_xlpm.office),
+_xlpm.growth,_xlpm.sales2016-_xlpm.sales2015,
+_xlpm.array,CHOOSE({1,2},_xlpm.office,_xlpm.growth),
+_xlfn._xlws.SORT(_xlpm.array,2,-1))</f>
+        <v>CHI</v>
+      </c>
+      <c r="N18" s="30">
+        <v>6742</v>
+      </c>
     </row>
     <row r="19" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M19" s="2"/>
-      <c r="N19" s="30"/>
+      <c r="M19" s="2" t="str">
+        <v>NYC</v>
+      </c>
+      <c r="N19" s="30">
+        <v>-3494</v>
+      </c>
     </row>
     <row r="20" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M20" s="2"/>
-      <c r="N20" s="30"/>
+      <c r="M20" s="2" t="str">
+        <v>BOS</v>
+      </c>
+      <c r="N20" s="30">
+        <v>-3861</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>